<commit_message>
Support dupliacte content by using title_hash - content_hash as TextID in excel file
</commit_message>
<xml_diff>
--- a/tests/expect_result/excel轉檔測試/excel欄位測試1_TextID_mapping.xlsx
+++ b/tests/expect_result/excel轉檔測試/excel欄位測試1_TextID_mapping.xlsx
@@ -448,108 +448,108 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1a50787db8</t>
+          <t>114091a778-1a50787db8</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>9066f1e71b</t>
+          <t>114091a778-9066f1e71b</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>341ce94b5d</t>
+          <t>196d11e6b8-341ce94b5d</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>a6b5cb57a3</t>
+          <t>196d11e6b8-a6b5cb57a3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>63b09e56e9</t>
+          <t>19fb0e96dd-63b09e56e9</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>63b09e56e9</t>
+          <t>19fb0e96dd-63b09e56e9</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>665ca36a3e</t>
+          <t>48aba86cb8-702980d58a</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>665ca36a3e</t>
+          <t>48aba86cb8-702980d58a</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>6a35e27a02</t>
+          <t>7d066011f6-6a35e27a02</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6a35e27a02</t>
+          <t>7d066011f6-6a35e27a02</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>702980d58a</t>
+          <t>8a8394d9eb-a4fafb4123</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>702980d58a</t>
+          <t>8a8394d9eb-a4fafb4123</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a4fafb4123</t>
+          <t>d5722a624b-ad620af736</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>a4fafb4123</t>
+          <t>d5722a624b-ad620af736</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>aa576e641b</t>
+          <t>d8499f5e39-aa576e641b</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>aa576e641b</t>
+          <t>d8499f5e39-aa576e641b</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ad620af736</t>
+          <t>e2e1425a6e-665ca36a3e</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ad620af736</t>
+          <t>e2e1425a6e-665ca36a3e</t>
         </is>
       </c>
     </row>

</xml_diff>